<commit_message>
tried to make sure the sim65m files have the 90 (ccw) rotation in the place files..jlcpcb apparently corrects the rotation from 0, so no big deal, but ATGM336N has 0 rotation, and SIM65M has 90. I check the pin 1 in the datasheet, they are just shown differently. the rotation fixes that
</commit_message>
<xml_diff>
--- a/pcb/tracker/v0.4_kbn/PickAndPlace_PCB1_2023-09-11_atgm336h-5n31.xlsx
+++ b/pcb/tracker/v0.4_kbn/PickAndPlace_PCB1_2023-09-11_atgm336h-5n31.xlsx
@@ -774,7 +774,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F6" activeCellId="0" sqref="F6"/>
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -886,7 +886,7 @@
         <v>8</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
seems like the original kazu placement had rotation 0 for atgm336 and it was always corrected to 180. fixed in _kbn.xlsx and _atgm336h-5n31.xlsx. Left the original kazu xlsx with rotation 0. jlcpcb apparently would fix to match pin 1? sim65m has different rotation to get pin 1 on pin1. I build with 0 and they fixed it. it should be 90 (already fixed). datasheets show top view different orientation, but pin 1 same name on both (etc on all other pins)
</commit_message>
<xml_diff>
--- a/pcb/tracker/v0.4_kbn/PickAndPlace_PCB1_2023-09-11_atgm336h-5n31.xlsx
+++ b/pcb/tracker/v0.4_kbn/PickAndPlace_PCB1_2023-09-11_atgm336h-5n31.xlsx
@@ -774,7 +774,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
+      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -886,7 +886,7 @@
         <v>8</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>0</v>
+        <v>180</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
need 180 deg rotation on u5. jlcpcb fixed the rotation  (ATGM336H)
</commit_message>
<xml_diff>
--- a/pcb/tracker/v0.4_kbn/PickAndPlace_PCB1_2023-09-11_atgm336h-5n31.xlsx
+++ b/pcb/tracker/v0.4_kbn/PickAndPlace_PCB1_2023-09-11_atgm336h-5n31.xlsx
@@ -774,7 +774,7 @@
   <dimension ref="A1:E1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H13" activeCellId="0" sqref="H13"/>
+      <selection pane="topLeft" activeCell="J17" activeCellId="0" sqref="J17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.8515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -886,7 +886,7 @@
         <v>8</v>
       </c>
       <c r="E6" s="3" t="n">
-        <v>180</v>
+        <v>0</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="13.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>